<commit_message>
format_header() w/ clean_header arg
</commit_message>
<xml_diff>
--- a/Reports/Example Clinical Report.xlsx
+++ b/Reports/Example Clinical Report.xlsx
@@ -18,49 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="47">
-  <si>
-    <t>client_id</t>
-  </si>
-  <si>
-    <t>doctor</t>
-  </si>
-  <si>
-    <t>cell_count</t>
-  </si>
-  <si>
-    <t>glucose_level</t>
-  </si>
-  <si>
-    <t>sucrose_level</t>
-  </si>
-  <si>
-    <t>procedure_cost</t>
-  </si>
-  <si>
-    <t>insurance_pymt</t>
-  </si>
-  <si>
-    <t>pct_paid</t>
-  </si>
-  <si>
-    <t>client_pay_pct</t>
-  </si>
-  <si>
-    <t>recovery_rate</t>
-  </si>
-  <si>
-    <t>birth_date</t>
-  </si>
-  <si>
-    <t>admit_date</t>
-  </si>
-  <si>
-    <t>chart_start</t>
-  </si>
-  <si>
-    <t>chart_end</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="52">
   <si>
     <t>Beckler</t>
   </si>
@@ -74,6 +32,48 @@
     <t>Example Client Data</t>
   </si>
   <si>
+    <t>Client Id</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>Cell Count</t>
+  </si>
+  <si>
+    <t>Glucose Level</t>
+  </si>
+  <si>
+    <t>Sucrose Level</t>
+  </si>
+  <si>
+    <t>Procedure Cost</t>
+  </si>
+  <si>
+    <t>Insurance Pymt</t>
+  </si>
+  <si>
+    <t>Pct Paid</t>
+  </si>
+  <si>
+    <t>Client Pay Pct</t>
+  </si>
+  <si>
+    <t>Recovery Rate</t>
+  </si>
+  <si>
+    <t>Birth Date</t>
+  </si>
+  <si>
+    <t>Admit Date</t>
+  </si>
+  <si>
+    <t>Chart Start</t>
+  </si>
+  <si>
+    <t>Chart End</t>
+  </si>
+  <si>
     <t>FY 2017-18</t>
   </si>
   <si>
@@ -158,7 +158,22 @@
     <t>Unique Clients by Department &amp; Gender (New Gender Classification Method)</t>
   </si>
   <si>
-    <t>Single DType Test</t>
+    <t>Clean Header Test</t>
+  </si>
+  <si>
+    <t>Fy 2017-18</t>
+  </si>
+  <si>
+    <t>Fy 2018-19</t>
+  </si>
+  <si>
+    <t>Fy 2019-2020</t>
+  </si>
+  <si>
+    <t>Fy 2020-21</t>
+  </si>
+  <si>
+    <t>Fy 2021-22</t>
   </si>
 </sst>
 </file>
@@ -661,51 +676,51 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="13" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="14" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="O3" s="15"/>
     </row>
@@ -714,7 +729,7 @@
         <v>545451</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>1232143</v>
@@ -759,7 +774,7 @@
         <v>78953</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
         <v>234</v>
@@ -804,7 +819,7 @@
         <v>136566</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
         <v>23422</v>
@@ -2986,230 +3001,782 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB7"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="15" width="10.7109375" style="1" customWidth="1"/>
-    <col min="2" max="16" width="9.7109375" style="1" customWidth="1"/>
-    <col min="3" max="17" width="11.7109375" style="1" customWidth="1"/>
-    <col min="4" max="18" width="14.7109375" style="1" customWidth="1"/>
-    <col min="5" max="19" width="14.7109375" style="1" customWidth="1"/>
-    <col min="6" max="20" width="15.7109375" style="1" customWidth="1"/>
-    <col min="7" max="21" width="15.7109375" style="1" customWidth="1"/>
-    <col min="8" max="22" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="23" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10" max="24" width="14.7109375" style="1" customWidth="1"/>
-    <col min="11" max="25" width="20.7109375" style="1" customWidth="1"/>
-    <col min="12" max="26" width="20.7109375" style="1" customWidth="1"/>
-    <col min="13" max="27" width="20.7109375" style="1" customWidth="1"/>
-    <col min="14" max="28" width="20.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:8">
       <c r="A1" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2491</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1601</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1898</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1722</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1601</v>
+      </c>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1758</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1346</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1162</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1208</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1406</v>
+      </c>
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1">
+        <v>229</v>
+      </c>
+      <c r="D6" s="1">
+        <v>251</v>
+      </c>
+      <c r="E6" s="1">
+        <v>213</v>
+      </c>
+      <c r="F6" s="1">
+        <v>333</v>
+      </c>
+      <c r="G6" s="1">
+        <v>222</v>
+      </c>
+      <c r="H6" s="15"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1">
+        <v>103</v>
+      </c>
+      <c r="D7" s="1">
+        <v>125</v>
+      </c>
+      <c r="E7" s="1">
+        <v>197</v>
+      </c>
+      <c r="F7" s="1">
+        <v>122</v>
+      </c>
+      <c r="G7" s="1">
+        <v>261</v>
+      </c>
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="1">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1">
+        <v>27</v>
+      </c>
+      <c r="E8" s="1">
+        <v>56</v>
+      </c>
+      <c r="F8" s="1">
+        <v>21</v>
+      </c>
+      <c r="G8" s="1">
+        <v>57</v>
+      </c>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="24">
+        <v>10</v>
+      </c>
+      <c r="D9" s="24">
+        <v>10</v>
+      </c>
+      <c r="E9" s="24">
+        <v>11</v>
+      </c>
+      <c r="F9" s="24">
+        <v>8</v>
+      </c>
+      <c r="G9" s="24">
+        <v>11</v>
+      </c>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1736</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1691</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1947</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2439</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1647</v>
+      </c>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1082</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1119</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1980</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1602</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1586</v>
+      </c>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="1">
+        <v>140</v>
+      </c>
+      <c r="D12" s="1">
+        <v>172</v>
+      </c>
+      <c r="E12" s="1">
+        <v>159</v>
+      </c>
+      <c r="F12" s="1">
+        <v>241</v>
+      </c>
+      <c r="G12" s="1">
+        <v>300</v>
+      </c>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="1">
+        <v>176</v>
+      </c>
+      <c r="D13" s="1">
+        <v>283</v>
+      </c>
+      <c r="E13" s="1">
+        <v>119</v>
+      </c>
+      <c r="F13" s="1">
+        <v>266</v>
+      </c>
+      <c r="G13" s="1">
+        <v>144</v>
+      </c>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="1">
+        <v>22</v>
+      </c>
+      <c r="D14" s="1">
+        <v>36</v>
+      </c>
+      <c r="E14" s="1">
+        <v>42</v>
+      </c>
+      <c r="F14" s="1">
+        <v>16</v>
+      </c>
+      <c r="G14" s="1">
+        <v>45</v>
+      </c>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="24">
+        <v>1</v>
+      </c>
+      <c r="D15" s="24">
+        <v>10</v>
+      </c>
+      <c r="E15" s="24">
+        <v>3</v>
+      </c>
+      <c r="F15" s="24">
+        <v>15</v>
+      </c>
+      <c r="G15" s="24">
+        <v>15</v>
+      </c>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1629</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1891</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2477</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1848</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1546</v>
+      </c>
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1891</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1246</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1032</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1712</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1761</v>
+      </c>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="1">
+        <v>205</v>
+      </c>
+      <c r="D18" s="1">
+        <v>204</v>
+      </c>
+      <c r="E18" s="1">
+        <v>178</v>
+      </c>
+      <c r="F18" s="1">
+        <v>261</v>
+      </c>
+      <c r="G18" s="1">
+        <v>224</v>
+      </c>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="1">
+        <v>103</v>
+      </c>
+      <c r="D19" s="1">
+        <v>93</v>
+      </c>
+      <c r="E19" s="1">
+        <v>279</v>
+      </c>
+      <c r="F19" s="1">
+        <v>284</v>
+      </c>
+      <c r="G19" s="1">
+        <v>102</v>
+      </c>
+      <c r="H19" s="15"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="1">
+        <v>11</v>
+      </c>
+      <c r="D20" s="1">
+        <v>39</v>
+      </c>
+      <c r="E20" s="1">
+        <v>37</v>
+      </c>
+      <c r="F20" s="1">
+        <v>44</v>
+      </c>
+      <c r="G20" s="1">
+        <v>31</v>
+      </c>
+      <c r="H20" s="15"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="24">
+        <v>4</v>
+      </c>
+      <c r="D21" s="24">
+        <v>5</v>
+      </c>
+      <c r="E21" s="24">
+        <v>7</v>
+      </c>
+      <c r="F21" s="24">
+        <v>2</v>
+      </c>
+      <c r="G21" s="24">
+        <v>5</v>
+      </c>
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1990</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1669</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2493</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1864</v>
+      </c>
+      <c r="G22" s="1">
+        <v>2200</v>
+      </c>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1760</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1067</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1406</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1193</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1382</v>
+      </c>
+      <c r="H23" s="15"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="1">
+        <v>333</v>
+      </c>
+      <c r="D24" s="1">
+        <v>148</v>
+      </c>
+      <c r="E24" s="1">
+        <v>288</v>
+      </c>
+      <c r="F24" s="1">
+        <v>284</v>
+      </c>
+      <c r="G24" s="1">
+        <v>333</v>
+      </c>
+      <c r="H24" s="15"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="1">
+        <v>263</v>
+      </c>
+      <c r="D25" s="1">
+        <v>113</v>
+      </c>
+      <c r="E25" s="1">
+        <v>253</v>
+      </c>
+      <c r="F25" s="1">
+        <v>149</v>
+      </c>
+      <c r="G25" s="1">
+        <v>129</v>
+      </c>
+      <c r="H25" s="15"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="1">
+        <v>46</v>
+      </c>
+      <c r="D26" s="1">
+        <v>52</v>
+      </c>
+      <c r="E26" s="1">
+        <v>35</v>
+      </c>
+      <c r="F26" s="1">
+        <v>10</v>
+      </c>
+      <c r="G26" s="1">
+        <v>51</v>
+      </c>
+      <c r="H26" s="15"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="24">
+        <v>15</v>
+      </c>
+      <c r="D27" s="24">
+        <v>13</v>
+      </c>
+      <c r="E27" s="24">
         <v>0</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="F27" s="24">
+        <v>10</v>
+      </c>
+      <c r="G27" s="24">
+        <v>11</v>
+      </c>
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2480</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1741</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1508</v>
+      </c>
+      <c r="F28" s="1">
+        <v>2189</v>
+      </c>
+      <c r="G28" s="1">
+        <v>2444</v>
+      </c>
+      <c r="H28" s="15"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1755</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1224</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1713</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1119</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1130</v>
+      </c>
+      <c r="H29" s="15"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="1">
+        <v>233</v>
+      </c>
+      <c r="D30" s="1">
+        <v>275</v>
+      </c>
+      <c r="E30" s="1">
+        <v>197</v>
+      </c>
+      <c r="F30" s="1">
+        <v>183</v>
+      </c>
+      <c r="G30" s="1">
+        <v>187</v>
+      </c>
+      <c r="H30" s="15"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="1">
+        <v>110</v>
+      </c>
+      <c r="D31" s="1">
+        <v>251</v>
+      </c>
+      <c r="E31" s="1">
+        <v>287</v>
+      </c>
+      <c r="F31" s="1">
+        <v>265</v>
+      </c>
+      <c r="G31" s="1">
+        <v>266</v>
+      </c>
+      <c r="H31" s="15"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="1">
+        <v>39</v>
+      </c>
+      <c r="D32" s="1">
+        <v>54</v>
+      </c>
+      <c r="E32" s="1">
+        <v>11</v>
+      </c>
+      <c r="F32" s="1">
+        <v>39</v>
+      </c>
+      <c r="G32" s="1">
+        <v>27</v>
+      </c>
+      <c r="H32" s="15"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="24">
+        <v>8</v>
+      </c>
+      <c r="D33" s="24">
+        <v>11</v>
+      </c>
+      <c r="E33" s="24">
+        <v>15</v>
+      </c>
+      <c r="F33" s="24">
+        <v>14</v>
+      </c>
+      <c r="G33" s="24">
         <v>1</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" s="15"/>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="1">
-        <v>545451</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1232143</v>
-      </c>
-      <c r="D4" s="1">
-        <v>12312.12</v>
-      </c>
-      <c r="E4" s="1">
-        <v>7564.234</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2347458</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2145115.54</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0.913803587</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0.086196413</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0.45</v>
-      </c>
-      <c r="K4" s="1">
-        <v>32066</v>
-      </c>
-      <c r="L4" s="1">
-        <v>36962</v>
-      </c>
-      <c r="M4" s="1">
-        <v>35981.23819444444</v>
-      </c>
-      <c r="N4" s="1">
-        <v>38911.65416666667</v>
-      </c>
-      <c r="O4" s="15"/>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="1">
-        <v>78953</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1">
-        <v>234</v>
-      </c>
-      <c r="D5" s="1">
-        <v>67563</v>
-      </c>
-      <c r="E5" s="1">
-        <v>54354.64</v>
-      </c>
-      <c r="F5" s="1">
-        <v>75893</v>
-      </c>
-      <c r="G5" s="1">
-        <v>54312.43</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0.7156447889999999</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0.284355211</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0.234235</v>
-      </c>
-      <c r="K5" s="1">
-        <v>33830</v>
-      </c>
-      <c r="L5" s="1">
-        <v>38233</v>
-      </c>
-      <c r="M5" s="1">
-        <v>37358.31597222222</v>
-      </c>
-      <c r="N5" s="1">
-        <v>42237.18888888889</v>
-      </c>
-      <c r="O5" s="15"/>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="1">
-        <v>136566</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1">
-        <v>23422</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2542.3</v>
-      </c>
-      <c r="E6" s="1">
-        <v>3242.1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>876</v>
-      </c>
-      <c r="G6" s="1">
-        <v>562.21</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0.641792237</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0.358207763</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0.3214</v>
-      </c>
-      <c r="K6" s="1">
-        <v>44135</v>
-      </c>
-      <c r="L6" s="1">
-        <v>44362</v>
-      </c>
-      <c r="M6" s="1">
-        <v>44178.57291666666</v>
-      </c>
-      <c r="N6" s="1">
-        <v>44632.30069444444</v>
-      </c>
-      <c r="O6" s="15"/>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
+      <c r="H33" s="15"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="A28:A33"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
create report with multindex data type setting
</commit_message>
<xml_diff>
--- a/Reports/Example Clinical Report.xlsx
+++ b/Reports/Example Clinical Report.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="66">
   <si>
     <t>Beckler</t>
   </si>
@@ -158,22 +158,64 @@
     <t>Unique Clients by Department &amp; Gender (New Gender Classification Method)</t>
   </si>
   <si>
-    <t>Clean Header Test</t>
-  </si>
-  <si>
-    <t>Fy 2017-18</t>
-  </si>
-  <si>
-    <t>Fy 2018-19</t>
-  </si>
-  <si>
-    <t>Fy 2019-2020</t>
-  </si>
-  <si>
-    <t>Fy 2020-21</t>
-  </si>
-  <si>
-    <t>Fy 2021-22</t>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>nonbinary</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>Set Multiindex Data Type Test</t>
+  </si>
+  <si>
+    <t>text_var</t>
+  </si>
+  <si>
+    <t>numeric_var</t>
+  </si>
+  <si>
+    <t>decimal_1_var</t>
+  </si>
+  <si>
+    <t>decimal_2_var</t>
+  </si>
+  <si>
+    <t>dollar_var</t>
+  </si>
+  <si>
+    <t>dollar_cents_var</t>
+  </si>
+  <si>
+    <t>percent_var</t>
+  </si>
+  <si>
+    <t>percent_1_var</t>
+  </si>
+  <si>
+    <t>percent_2_var</t>
+  </si>
+  <si>
+    <t>date_var</t>
+  </si>
+  <si>
+    <t>date_alt_var</t>
+  </si>
+  <si>
+    <t>datetime_var</t>
+  </si>
+  <si>
+    <t>datetime_alt_var</t>
   </si>
 </sst>
 </file>
@@ -194,6 +236,16 @@
     <numFmt numFmtId="174" formatCode="yyyy-mm-dd h:mm"/>
     <numFmt numFmtId="175" formatCode="m/d/yyyy h:mm AM/PM"/>
     <numFmt numFmtId="164" formatCode="#,##0"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="$#,##0"/>
+    <numFmt numFmtId="168" formatCode="$#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="0%"/>
+    <numFmt numFmtId="170" formatCode="0.0%"/>
+    <numFmt numFmtId="171" formatCode="0.00%"/>
+    <numFmt numFmtId="172" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="173" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="175" formatCode="m/d/yyyy h:mm AM/PM"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -313,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -358,6 +410,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3001,22 +3064,35 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" customWidth="1"/>
+    <col min="15" max="15" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:16">
       <c r="A1" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="20" t="s">
         <v>23</v>
       </c>
@@ -3024,758 +3100,500 @@
         <v>31</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="15"/>
-    </row>
-    <row r="4" spans="1:8">
+        <v>57</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="P3" s="15"/>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="21" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2491</v>
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
       </c>
       <c r="D4" s="1">
-        <v>1601</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1898</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1722</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1601</v>
-      </c>
-      <c r="H4" s="15"/>
-    </row>
-    <row r="5" spans="1:8">
+        <v>1232143</v>
+      </c>
+      <c r="E4" s="2">
+        <v>12312.12</v>
+      </c>
+      <c r="F4" s="3">
+        <v>7564.234</v>
+      </c>
+      <c r="G4" s="4">
+        <v>2347458</v>
+      </c>
+      <c r="H4" s="5">
+        <v>234.52</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0.123</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0.546542</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="L4" s="9">
+        <v>36597</v>
+      </c>
+      <c r="M4" s="10">
+        <v>32066</v>
+      </c>
+      <c r="N4" s="9">
+        <v>35981.23819444444</v>
+      </c>
+      <c r="O4" s="12">
+        <v>38911.65416666667</v>
+      </c>
+      <c r="P4" s="15"/>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="21" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1758</v>
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
       </c>
       <c r="D5" s="1">
-        <v>1346</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1162</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1208</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1406</v>
-      </c>
-      <c r="H5" s="15"/>
-    </row>
-    <row r="6" spans="1:8">
+        <v>234</v>
+      </c>
+      <c r="E5" s="2">
+        <v>67563</v>
+      </c>
+      <c r="F5" s="3">
+        <v>54354.64</v>
+      </c>
+      <c r="G5" s="4">
+        <v>4564</v>
+      </c>
+      <c r="H5" s="5">
+        <v>2345115.54</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0.63434</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.32</v>
+      </c>
+      <c r="K5" s="8">
+        <v>0.234235</v>
+      </c>
+      <c r="L5" s="9">
+        <v>33830</v>
+      </c>
+      <c r="M5" s="10">
+        <v>38233</v>
+      </c>
+      <c r="N5" s="9">
+        <v>38819.31597222222</v>
+      </c>
+      <c r="O5" s="12">
+        <v>42237.18888888889</v>
+      </c>
+      <c r="P5" s="15"/>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="1">
-        <v>229</v>
-      </c>
-      <c r="D6" s="1">
-        <v>251</v>
-      </c>
-      <c r="E6" s="1">
-        <v>213</v>
-      </c>
-      <c r="F6" s="1">
-        <v>333</v>
-      </c>
-      <c r="G6" s="1">
-        <v>222</v>
-      </c>
-      <c r="H6" s="15"/>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="B6" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="24">
+        <v>23422</v>
+      </c>
+      <c r="E6" s="27">
+        <v>2542.3</v>
+      </c>
+      <c r="F6" s="28">
+        <v>3242.1</v>
+      </c>
+      <c r="G6" s="29">
+        <v>876</v>
+      </c>
+      <c r="H6" s="30">
+        <v>54312.43</v>
+      </c>
+      <c r="I6" s="31">
+        <v>0.9</v>
+      </c>
+      <c r="J6" s="32">
+        <v>0.912</v>
+      </c>
+      <c r="K6" s="33">
+        <v>0.3214</v>
+      </c>
+      <c r="L6" s="34">
+        <v>44135</v>
+      </c>
+      <c r="M6" s="35">
+        <v>44362</v>
+      </c>
+      <c r="N6" s="34">
+        <v>41256.57291666666</v>
+      </c>
+      <c r="O6" s="36">
+        <v>43536.30069444444</v>
+      </c>
+      <c r="P6" s="15"/>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="1">
-        <v>103</v>
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
       </c>
       <c r="D7" s="1">
-        <v>125</v>
-      </c>
-      <c r="E7" s="1">
-        <v>197</v>
-      </c>
-      <c r="F7" s="1">
-        <v>122</v>
-      </c>
-      <c r="G7" s="1">
-        <v>261</v>
-      </c>
-      <c r="H7" s="15"/>
-    </row>
-    <row r="8" spans="1:8">
+        <v>234</v>
+      </c>
+      <c r="E7" s="2">
+        <v>67563</v>
+      </c>
+      <c r="F7" s="3">
+        <v>54354.64</v>
+      </c>
+      <c r="G7" s="4">
+        <v>4564</v>
+      </c>
+      <c r="H7" s="5">
+        <v>2345115.54</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0.63434</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0.32</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0.234235</v>
+      </c>
+      <c r="L7" s="9">
+        <v>33830</v>
+      </c>
+      <c r="M7" s="10">
+        <v>38233</v>
+      </c>
+      <c r="N7" s="9">
+        <v>38819.31597222222</v>
+      </c>
+      <c r="O7" s="12">
+        <v>42237.18888888889</v>
+      </c>
+      <c r="P7" s="15"/>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="1">
-        <v>39</v>
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
       </c>
       <c r="D8" s="1">
-        <v>27</v>
-      </c>
-      <c r="E8" s="1">
-        <v>56</v>
-      </c>
-      <c r="F8" s="1">
-        <v>21</v>
-      </c>
-      <c r="G8" s="1">
-        <v>57</v>
-      </c>
-      <c r="H8" s="15"/>
-    </row>
-    <row r="9" spans="1:8">
+        <v>23422</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2542.3</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3242.1</v>
+      </c>
+      <c r="G8" s="4">
+        <v>876</v>
+      </c>
+      <c r="H8" s="5">
+        <v>54312.43</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0.912</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0.3214</v>
+      </c>
+      <c r="L8" s="9">
+        <v>44135</v>
+      </c>
+      <c r="M8" s="10">
+        <v>44362</v>
+      </c>
+      <c r="N8" s="9">
+        <v>41256.57291666666</v>
+      </c>
+      <c r="O8" s="12">
+        <v>43536.30069444444</v>
+      </c>
+      <c r="P8" s="15"/>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="24">
-        <v>10</v>
+        <v>48</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>49</v>
       </c>
       <c r="D9" s="24">
-        <v>10</v>
-      </c>
-      <c r="E9" s="24">
-        <v>11</v>
-      </c>
-      <c r="F9" s="24">
-        <v>8</v>
-      </c>
-      <c r="G9" s="24">
-        <v>11</v>
-      </c>
-      <c r="H9" s="15"/>
-    </row>
-    <row r="10" spans="1:8">
+        <v>1232143</v>
+      </c>
+      <c r="E9" s="27">
+        <v>12312.12</v>
+      </c>
+      <c r="F9" s="28">
+        <v>7564.234</v>
+      </c>
+      <c r="G9" s="29">
+        <v>2347458</v>
+      </c>
+      <c r="H9" s="30">
+        <v>234.52</v>
+      </c>
+      <c r="I9" s="31">
+        <v>0.123</v>
+      </c>
+      <c r="J9" s="32">
+        <v>0.546542</v>
+      </c>
+      <c r="K9" s="33">
+        <v>0.45</v>
+      </c>
+      <c r="L9" s="34">
+        <v>36597</v>
+      </c>
+      <c r="M9" s="35">
+        <v>32066</v>
+      </c>
+      <c r="N9" s="34">
+        <v>35981.23819444444</v>
+      </c>
+      <c r="O9" s="36">
+        <v>38911.65416666667</v>
+      </c>
+      <c r="P9" s="15"/>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" s="21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1736</v>
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
       </c>
       <c r="D10" s="1">
-        <v>1691</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1947</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2439</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1647</v>
-      </c>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" spans="1:8">
+        <v>23422</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2542.3</v>
+      </c>
+      <c r="F10" s="3">
+        <v>3242.1</v>
+      </c>
+      <c r="G10" s="4">
+        <v>876</v>
+      </c>
+      <c r="H10" s="5">
+        <v>54312.43</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="J10" s="7">
+        <v>0.912</v>
+      </c>
+      <c r="K10" s="8">
+        <v>0.3214</v>
+      </c>
+      <c r="L10" s="9">
+        <v>44135</v>
+      </c>
+      <c r="M10" s="10">
+        <v>44362</v>
+      </c>
+      <c r="N10" s="9">
+        <v>41256.57291666666</v>
+      </c>
+      <c r="O10" s="12">
+        <v>43536.30069444444</v>
+      </c>
+      <c r="P10" s="15"/>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" s="21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1082</v>
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
       </c>
       <c r="D11" s="1">
-        <v>1119</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1980</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1602</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1586</v>
-      </c>
-      <c r="H11" s="15"/>
-    </row>
-    <row r="12" spans="1:8">
+        <v>1232143</v>
+      </c>
+      <c r="E11" s="2">
+        <v>12312.12</v>
+      </c>
+      <c r="F11" s="3">
+        <v>7564.234</v>
+      </c>
+      <c r="G11" s="4">
+        <v>2347458</v>
+      </c>
+      <c r="H11" s="5">
+        <v>234.52</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.123</v>
+      </c>
+      <c r="J11" s="7">
+        <v>0.546542</v>
+      </c>
+      <c r="K11" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="L11" s="9">
+        <v>36597</v>
+      </c>
+      <c r="M11" s="10">
+        <v>32066</v>
+      </c>
+      <c r="N11" s="9">
+        <v>35981.23819444444</v>
+      </c>
+      <c r="O11" s="12">
+        <v>38911.65416666667</v>
+      </c>
+      <c r="P11" s="15"/>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="1">
-        <v>140</v>
-      </c>
-      <c r="D12" s="1">
-        <v>172</v>
-      </c>
-      <c r="E12" s="1">
-        <v>159</v>
-      </c>
-      <c r="F12" s="1">
-        <v>241</v>
-      </c>
-      <c r="G12" s="1">
-        <v>300</v>
-      </c>
-      <c r="H12" s="15"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="1">
-        <v>176</v>
-      </c>
-      <c r="D13" s="1">
-        <v>283</v>
-      </c>
-      <c r="E13" s="1">
-        <v>119</v>
-      </c>
-      <c r="F13" s="1">
-        <v>266</v>
-      </c>
-      <c r="G13" s="1">
-        <v>144</v>
-      </c>
-      <c r="H13" s="15"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="1">
-        <v>22</v>
-      </c>
-      <c r="D14" s="1">
-        <v>36</v>
-      </c>
-      <c r="E14" s="1">
-        <v>42</v>
-      </c>
-      <c r="F14" s="1">
-        <v>16</v>
-      </c>
-      <c r="G14" s="1">
-        <v>45</v>
-      </c>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="24">
-        <v>1</v>
-      </c>
-      <c r="D15" s="24">
-        <v>10</v>
-      </c>
-      <c r="E15" s="24">
-        <v>3</v>
-      </c>
-      <c r="F15" s="24">
-        <v>15</v>
-      </c>
-      <c r="G15" s="24">
-        <v>15</v>
-      </c>
-      <c r="H15" s="15"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1629</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1891</v>
-      </c>
-      <c r="E16" s="1">
-        <v>2477</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1848</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1546</v>
-      </c>
-      <c r="H16" s="15"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1891</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1246</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1032</v>
-      </c>
-      <c r="F17" s="1">
-        <v>1712</v>
-      </c>
-      <c r="G17" s="1">
-        <v>1761</v>
-      </c>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="1">
-        <v>205</v>
-      </c>
-      <c r="D18" s="1">
-        <v>204</v>
-      </c>
-      <c r="E18" s="1">
-        <v>178</v>
-      </c>
-      <c r="F18" s="1">
-        <v>261</v>
-      </c>
-      <c r="G18" s="1">
-        <v>224</v>
-      </c>
-      <c r="H18" s="15"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="1">
-        <v>103</v>
-      </c>
-      <c r="D19" s="1">
-        <v>93</v>
-      </c>
-      <c r="E19" s="1">
-        <v>279</v>
-      </c>
-      <c r="F19" s="1">
-        <v>284</v>
-      </c>
-      <c r="G19" s="1">
-        <v>102</v>
-      </c>
-      <c r="H19" s="15"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="1">
-        <v>11</v>
-      </c>
-      <c r="D20" s="1">
-        <v>39</v>
-      </c>
-      <c r="E20" s="1">
-        <v>37</v>
-      </c>
-      <c r="F20" s="1">
-        <v>44</v>
-      </c>
-      <c r="G20" s="1">
-        <v>31</v>
-      </c>
-      <c r="H20" s="15"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="24">
-        <v>4</v>
-      </c>
-      <c r="D21" s="24">
-        <v>5</v>
-      </c>
-      <c r="E21" s="24">
-        <v>7</v>
-      </c>
-      <c r="F21" s="24">
-        <v>2</v>
-      </c>
-      <c r="G21" s="24">
-        <v>5</v>
-      </c>
-      <c r="H21" s="15"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1990</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1669</v>
-      </c>
-      <c r="E22" s="1">
-        <v>2493</v>
-      </c>
-      <c r="F22" s="1">
-        <v>1864</v>
-      </c>
-      <c r="G22" s="1">
-        <v>2200</v>
-      </c>
-      <c r="H22" s="15"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1760</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1067</v>
-      </c>
-      <c r="E23" s="1">
-        <v>1406</v>
-      </c>
-      <c r="F23" s="1">
-        <v>1193</v>
-      </c>
-      <c r="G23" s="1">
-        <v>1382</v>
-      </c>
-      <c r="H23" s="15"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="1">
-        <v>333</v>
-      </c>
-      <c r="D24" s="1">
-        <v>148</v>
-      </c>
-      <c r="E24" s="1">
-        <v>288</v>
-      </c>
-      <c r="F24" s="1">
-        <v>284</v>
-      </c>
-      <c r="G24" s="1">
-        <v>333</v>
-      </c>
-      <c r="H24" s="15"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="1">
-        <v>263</v>
-      </c>
-      <c r="D25" s="1">
-        <v>113</v>
-      </c>
-      <c r="E25" s="1">
-        <v>253</v>
-      </c>
-      <c r="F25" s="1">
-        <v>149</v>
-      </c>
-      <c r="G25" s="1">
-        <v>129</v>
-      </c>
-      <c r="H25" s="15"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="1">
-        <v>46</v>
-      </c>
-      <c r="D26" s="1">
-        <v>52</v>
-      </c>
-      <c r="E26" s="1">
-        <v>35</v>
-      </c>
-      <c r="F26" s="1">
-        <v>10</v>
-      </c>
-      <c r="G26" s="1">
-        <v>51</v>
-      </c>
-      <c r="H26" s="15"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="24">
-        <v>15</v>
-      </c>
-      <c r="D27" s="24">
-        <v>13</v>
-      </c>
-      <c r="E27" s="24">
-        <v>0</v>
-      </c>
-      <c r="F27" s="24">
-        <v>10</v>
-      </c>
-      <c r="G27" s="24">
-        <v>11</v>
-      </c>
-      <c r="H27" s="15"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="1">
-        <v>2480</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1741</v>
-      </c>
-      <c r="E28" s="1">
-        <v>1508</v>
-      </c>
-      <c r="F28" s="1">
-        <v>2189</v>
-      </c>
-      <c r="G28" s="1">
-        <v>2444</v>
-      </c>
-      <c r="H28" s="15"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1755</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1224</v>
-      </c>
-      <c r="E29" s="1">
-        <v>1713</v>
-      </c>
-      <c r="F29" s="1">
-        <v>1119</v>
-      </c>
-      <c r="G29" s="1">
-        <v>1130</v>
-      </c>
-      <c r="H29" s="15"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="1">
-        <v>233</v>
-      </c>
-      <c r="D30" s="1">
-        <v>275</v>
-      </c>
-      <c r="E30" s="1">
-        <v>197</v>
-      </c>
-      <c r="F30" s="1">
-        <v>183</v>
-      </c>
-      <c r="G30" s="1">
-        <v>187</v>
-      </c>
-      <c r="H30" s="15"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="1">
-        <v>110</v>
-      </c>
-      <c r="D31" s="1">
-        <v>251</v>
-      </c>
-      <c r="E31" s="1">
-        <v>287</v>
-      </c>
-      <c r="F31" s="1">
-        <v>265</v>
-      </c>
-      <c r="G31" s="1">
-        <v>266</v>
-      </c>
-      <c r="H31" s="15"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="1">
-        <v>39</v>
-      </c>
-      <c r="D32" s="1">
-        <v>54</v>
-      </c>
-      <c r="E32" s="1">
-        <v>11</v>
-      </c>
-      <c r="F32" s="1">
-        <v>39</v>
-      </c>
-      <c r="G32" s="1">
-        <v>27</v>
-      </c>
-      <c r="H32" s="15"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="24">
-        <v>8</v>
-      </c>
-      <c r="D33" s="24">
-        <v>11</v>
-      </c>
-      <c r="E33" s="24">
-        <v>15</v>
-      </c>
-      <c r="F33" s="24">
-        <v>14</v>
-      </c>
-      <c r="G33" s="24">
-        <v>1</v>
-      </c>
-      <c r="H33" s="15"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
+      <c r="B12" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="24">
+        <v>234</v>
+      </c>
+      <c r="E12" s="27">
+        <v>67563</v>
+      </c>
+      <c r="F12" s="28">
+        <v>54354.64</v>
+      </c>
+      <c r="G12" s="29">
+        <v>4564</v>
+      </c>
+      <c r="H12" s="30">
+        <v>2345115.54</v>
+      </c>
+      <c r="I12" s="31">
+        <v>0.63434</v>
+      </c>
+      <c r="J12" s="32">
+        <v>0.32</v>
+      </c>
+      <c r="K12" s="33">
+        <v>0.234235</v>
+      </c>
+      <c r="L12" s="34">
+        <v>33830</v>
+      </c>
+      <c r="M12" s="35">
+        <v>38233</v>
+      </c>
+      <c r="N12" s="34">
+        <v>38819.31597222222</v>
+      </c>
+      <c r="O12" s="36">
+        <v>42237.18888888889</v>
+      </c>
+      <c r="P12" s="15"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="A28:A33"/>
+  <mergeCells count="3">
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A10:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>